<commit_message>
added options for Abx0_6 and Abx6_12
</commit_message>
<xml_diff>
--- a/data_record.xlsx
+++ b/data_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leahbriscoe/Documents/MicroBatch/microbatch_vc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8DB98E-EB5D-784A-A3FD-8553B295D291}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A13C15B-58BA-C643-BBEF-CFDABA2EB3E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12840" yWindow="460" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{F8BBA8BF-065C-B746-B1EF-04D62E9AF879}"/>
+    <workbookView xWindow="17380" yWindow="460" windowWidth="27640" windowHeight="19860" activeTab="1" xr2:uid="{F8BBA8BF-065C-B746-B1EF-04D62E9AF879}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="79">
   <si>
     <t>best method (naïve bayes)</t>
   </si>
@@ -226,14 +226,67 @@
   </si>
   <si>
     <t xml:space="preserve"> 143     352  CRC    318 </t>
+  </si>
+  <si>
+    <t>colorectal cancer</t>
+  </si>
+  <si>
+    <t>Gibbons et al</t>
+  </si>
+  <si>
+    <t>OTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wirbel et al. </t>
+  </si>
+  <si>
+    <t>Amplicon</t>
+  </si>
+  <si>
+    <t>Amplicon/WGS</t>
+  </si>
+  <si>
+    <t>WGS</t>
+  </si>
+  <si>
+    <t>16S</t>
+  </si>
+  <si>
+    <t>16S?</t>
+  </si>
+  <si>
+    <t>Alcohol consumption</t>
+  </si>
+  <si>
+    <t>Diet</t>
+  </si>
+  <si>
+    <t>Type II Diabetes</t>
+  </si>
+  <si>
+    <t>WGS?</t>
+  </si>
+  <si>
+    <t>7 datasets</t>
+  </si>
+  <si>
+    <t>16 Phenotypes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -253,8 +306,23 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,8 +341,20 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -282,15 +362,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,246 +934,623 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428FAFB1-A660-CB43-AFE3-FA4CDEF4FAC2}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="30.5" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="7" max="7" width="18.5" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="32.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="24" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15" style="3" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" style="3"/>
+    <col min="8" max="8" width="18.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="8">
         <f>7293+17610</f>
         <v>24903</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="5">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" s="4" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F3">
+      <c r="E3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="8">
+        <f t="shared" ref="F3:F5" si="0">7293+17610</f>
+        <v>24903</v>
+      </c>
+      <c r="G3" s="8">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="11">
+        <f t="shared" si="0"/>
+        <v>24903</v>
+      </c>
+      <c r="G4" s="11">
+        <v>1</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="0"/>
+        <v>24903</v>
+      </c>
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" s="4" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E5">
+      <c r="C7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="8">
         <f>143+352+318</f>
         <v>813</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G7" s="8">
+        <v>6</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I7" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J7" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="8" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" s="4" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="8">
+        <f>143+352+318</f>
+        <v>813</v>
+      </c>
+      <c r="G9" s="8">
+        <v>6</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" s="4" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8">
+        <v>3</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B15" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C15" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E15" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E9">
+      <c r="F15" s="11">
         <v>1895</v>
       </c>
-      <c r="F9">
+      <c r="G15" s="11">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H15" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I15" s="11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
+      <c r="J15" s="11"/>
+    </row>
+    <row r="16" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E16" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E10">
+      <c r="F16" s="11">
         <v>1895</v>
       </c>
-      <c r="F10">
+      <c r="G16" s="11">
         <v>1</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H16" s="11"/>
+      <c r="I16" s="11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E17" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E11">
+      <c r="F17" s="11">
         <v>1895</v>
       </c>
-      <c r="F11">
+      <c r="G17" s="11">
         <v>1</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H17" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I17" s="11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E18" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E12">
+      <c r="F18" s="11">
         <v>1895</v>
       </c>
-      <c r="F12">
+      <c r="G18" s="11">
         <v>1</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H18" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I18" s="11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="J18" s="11"/>
+    </row>
+    <row r="19" spans="1:10" ht="10" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+    </row>
+    <row r="20" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B20" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C20" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E20" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E14">
+      <c r="F20" s="11">
         <v>2528</v>
       </c>
-      <c r="F14">
+      <c r="G20" s="11">
         <v>2</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H20" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I20" s="11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="1:10" ht="41" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E21" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E15">
+      <c r="F21" s="11">
         <v>2528</v>
       </c>
-      <c r="F15">
+      <c r="G21" s="11">
         <v>2</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H21" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I21" s="11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E22" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E16">
+      <c r="F22" s="11">
         <v>2528</v>
       </c>
-      <c r="F16">
+      <c r="G22" s="11">
         <v>2</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H22" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I22" s="11" t="s">
         <v>43</v>
       </c>
+      <c r="J22" s="11"/>
+    </row>
+    <row r="23" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+    </row>
+    <row r="24" spans="1:10" s="4" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="8">
+        <v>508</v>
+      </c>
+      <c r="G24" s="8">
+        <v>2</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+    </row>
+    <row r="26" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+    </row>
+    <row r="29" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more parameters in RF
</commit_message>
<xml_diff>
--- a/data_record.xlsx
+++ b/data_record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leahbriscoe/Documents/MicroBatch/microbatch_vc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACBDE6F-4F6F-AF43-B278-795D1CA72070}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F71ED8-887C-254E-A22E-403CF3682E8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="460" windowWidth="27640" windowHeight="19860" activeTab="1" xr2:uid="{F8BBA8BF-065C-B746-B1EF-04D62E9AF879}"/>
+    <workbookView xWindow="1080" yWindow="460" windowWidth="27640" windowHeight="19860" activeTab="1" xr2:uid="{F8BBA8BF-065C-B746-B1EF-04D62E9AF879}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -336,7 +336,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,6 +364,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDE5D8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -439,12 +445,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFDE5D8"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -943,6 +963,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -950,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428FAFB1-A660-CB43-AFE3-FA4CDEF4FAC2}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1136,7 +1157,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="4" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="4" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>60</v>
       </c>
@@ -1181,7 +1202,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
     </row>
-    <row r="10" spans="1:10" s="4" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="4" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>60</v>
       </c>
@@ -1299,7 +1320,7 @@
       <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -1328,27 +1349,27 @@
       </c>
       <c r="J16" s="11"/>
     </row>
-    <row r="17" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11" t="s">
+    <row r="17" spans="1:10" s="14" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="13">
         <v>1895</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="13">
         <v>1</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11" t="s">
+      <c r="H17" s="13"/>
+      <c r="I17" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="11"/>
+      <c r="J17" s="13"/>
     </row>
     <row r="18" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
@@ -1595,5 +1616,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>